<commit_message>
found bug in patient view/entity report patient fixed it and updated testplan
</commit_message>
<xml_diff>
--- a/test/testplan.xlsx
+++ b/test/testplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="117">
   <si>
     <t>Preparation</t>
   </si>
@@ -378,6 +378,42 @@
   </si>
   <si>
     <t xml:space="preserve">Does the table disapear? </t>
+  </si>
+  <si>
+    <t>Entity report patient</t>
+  </si>
+  <si>
+    <t>Go to the data tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the entityreport button </t>
+  </si>
+  <si>
+    <t>A patient view like screen should show</t>
+  </si>
+  <si>
+    <t>Try to search in the table</t>
+  </si>
+  <si>
+    <t>Does it work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try to download </t>
+  </si>
+  <si>
+    <t>Does a file download with the name: patient_data_*patient name*.pdf?</t>
+  </si>
+  <si>
+    <t>Check the file</t>
+  </si>
+  <si>
+    <t>Does it contain the content of the patient table? (yes genotype shows very ugly)</t>
+  </si>
+  <si>
+    <t>Now once go the the patient view again and select the same patient as you selected in the entity report</t>
+  </si>
+  <si>
+    <t>Does everything appear the same as before?</t>
   </si>
 </sst>
 </file>
@@ -457,8 +493,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -519,7 +561,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -543,6 +585,9 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -566,6 +611,9 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -895,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1406,6 +1454,59 @@
         <v>104</v>
       </c>
     </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
fixed bug in gene view, count was off by selection
</commit_message>
<xml_diff>
--- a/test/testplan.xlsx
+++ b/test/testplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="119">
   <si>
     <t>Preparation</t>
   </si>
@@ -414,6 +414,12 @@
   </si>
   <si>
     <t>Does everything appear the same as before?</t>
+  </si>
+  <si>
+    <t>Make sure d3.js is in the header of MOLGENIS, above jQuery!</t>
+  </si>
+  <si>
+    <t>&lt;script src="https://cdnjs.cloudflare.com/ajax/libs/d3/3.5.6/d3.min.js" charset="utf-8"&gt;&lt;/script&gt;</t>
   </si>
 </sst>
 </file>
@@ -493,8 +499,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -561,7 +569,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -588,6 +596,7 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -614,6 +623,7 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -943,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1025,485 +1035,493 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:2" ht="15">
+      <c r="A13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:2" ht="26">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="26">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="26">
       <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" ht="26">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" ht="26">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="26">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" ht="26">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" ht="26">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:2" ht="26">
       <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="26">
+      <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="26">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:2" ht="26">
+      <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" ht="39">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" ht="39">
+      <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="26">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:2" ht="26">
+      <c r="A33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="1"/>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" ht="26">
-      <c r="A35" s="5" t="s">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" ht="26">
+      <c r="A36" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="26">
-      <c r="A51" s="5" t="s">
+    <row r="52" spans="1:2" ht="26">
+      <c r="A52" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B52" s="5" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="5"/>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="3" t="s">
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="B61" s="3"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="26">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:2" ht="26">
+      <c r="A69" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B69" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:2">
+      <c r="A70" s="1" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="26">
-      <c r="A70" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="26">
       <c r="A71" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="26">
+      <c r="A72" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B72" s="5" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="3" t="s">
+    <row r="76" spans="1:2">
+      <c r="A76" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="B76" s="3"/>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="26">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:2" ht="26">
+      <c r="A79" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B79" s="5" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="3" t="s">
+    <row r="82" spans="1:2">
+      <c r="A82" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="B82" s="3"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
everything was broke in last I guess, fixed...
</commit_message>
<xml_diff>
--- a/test/testplan.xlsx
+++ b/test/testplan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="119">
   <si>
     <t>Preparation</t>
   </si>
@@ -33,9 +33,6 @@
     <t xml:space="preserve">Go to the Data Explorer and open the FreemarkerTemplate table </t>
   </si>
   <si>
-    <t>Make a new tempate and paste the content of the downloaded ftl file inside the template</t>
-  </si>
-  <si>
     <t>Call the template: view-test-entitiesreport.ftl</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
   </si>
   <si>
     <t>Scroll down to reports</t>
-  </si>
-  <si>
-    <t>Typ in this in the input box: chromosome6_a_c:test,chromome6_d_h:test,chromome_i_L,chromosome6_array</t>
   </si>
   <si>
     <r>
@@ -73,9 +67,6 @@
     </r>
   </si>
   <si>
-    <t>Upload the downloaded ftl files to MOLGENIS</t>
-  </si>
-  <si>
     <t>Click on "Save changes"</t>
   </si>
   <si>
@@ -423,6 +414,12 @@
   </si>
   <si>
     <t xml:space="preserve">Put the patient view ftl in the freemarkertemplate table in the dataexplorer with this names: view-entityreport-specific-*questionnairepart* </t>
+  </si>
+  <si>
+    <t>Typ in this in the input box: chromosome6_a_c:test,chromome6_d_h:test,chromome_i_L:test,chromosome6_array:test</t>
+  </si>
+  <si>
+    <t>Make a new tempate and paste the content of the downloaded ftl (functionality_tabs_v2.ftl) file inside the template</t>
   </si>
 </sst>
 </file>
@@ -962,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -988,20 +985,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:2" ht="52">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1011,530 +1006,530 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15">
       <c r="A13" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="26">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="26">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="26">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" ht="26">
       <c r="A20" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="26">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:2" ht="26">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="26">
       <c r="A31" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="26">
       <c r="A32" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2" ht="39">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="26">
       <c r="A34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:2" ht="26">
       <c r="A37" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="26">
       <c r="A53" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="26">
       <c r="A70" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="26">
       <c r="A72" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="26">
       <c r="A73" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B77" s="3"/>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="26">
       <c r="A80" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B83" s="3"/>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The whole phenotype of a patient can be shown in the phenotype view by clicking on a patient name
</commit_message>
<xml_diff>
--- a/test/testplan.xlsx
+++ b/test/testplan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="121">
   <si>
     <t>Preparation</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>Make a new tempate and paste the content of the downloaded ftl (functionality_tabs_v2.ftl) file inside the template</t>
+  </si>
+  <si>
+    <t>Click on a name of a patient next to the bar</t>
+  </si>
+  <si>
+    <t>A div should appear with the whole phenotype of the patient. This div is resizable and draggable.</t>
   </si>
 </sst>
 </file>
@@ -499,8 +505,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -571,7 +579,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -600,6 +608,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -628,6 +637,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -957,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1340,195 +1350,203 @@
       <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="B63" s="3"/>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="26">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:2" ht="26">
+      <c r="A71" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B71" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="26">
-      <c r="A72" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="26">
       <c r="A73" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="26">
+      <c r="A74" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B74" s="5" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="3" t="s">
+    <row r="78" spans="1:2">
+      <c r="A78" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="B78" s="3"/>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="26">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:2" ht="26">
+      <c r="A81" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="3" t="s">
+    <row r="84" spans="1:2">
+      <c r="A84" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added testfiles and updated testplan
</commit_message>
<xml_diff>
--- a/test/testplan.xlsx
+++ b/test/testplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,7 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Go to https://github.com/marikaris/ChromosomeView and download the xlsx files from the testFiles directory</t>
-  </si>
-  <si>
     <t xml:space="preserve">Go to the Data Explorer and open the FreemarkerTemplate table </t>
-  </si>
-  <si>
-    <t>Call the template: view-test-entitiesreport.ftl</t>
   </si>
   <si>
     <t>Go to settings (the gear right above the page)</t>
@@ -91,9 +85,6 @@
     <t>A dropdown appears with the list of patients you created</t>
   </si>
   <si>
-    <t>Fill in all three questionnaire parts and a Chromosome 6 Array in for 4 patients</t>
-  </si>
-  <si>
     <t>Single patient view</t>
   </si>
   <si>
@@ -131,12 +122,6 @@
   </si>
   <si>
     <t>Click on "Search"</t>
-  </si>
-  <si>
-    <t>Note 3 things : 
-1. Use four different aberrations (types and start and stop different). 
-2. For the same patient, use in all parts the same owner username. 
-3. The start and stop location in Hg19 should be between 0 and 170805979</t>
   </si>
   <si>
     <t>The table with data of the patients of this part of the questionnaire will show 
@@ -404,9 +389,6 @@
     <t>Does everything appear the same as before?</t>
   </si>
   <si>
-    <t>Make sure d3.js is in the header of MOLGENIS, above jQuery!</t>
-  </si>
-  <si>
     <t>&lt;script src="https://cdnjs.cloudflare.com/ajax/libs/d3/3.5.6/d3.min.js" charset="utf-8"&gt;&lt;/script&gt;</t>
   </si>
   <si>
@@ -419,13 +401,28 @@
     <t>Typ in this in the input box: chromosome6_a_c:test,chromome6_d_h:test,chromome_i_L:test,chromosome6_array:test</t>
   </si>
   <si>
-    <t>Make a new tempate and paste the content of the downloaded ftl (functionality_tabs_v2.ftl) file inside the template</t>
-  </si>
-  <si>
     <t>Click on a name of a patient next to the bar</t>
   </si>
   <si>
     <t>A div should appear with the whole phenotype of the patient. This div is resizable and draggable.</t>
+  </si>
+  <si>
+    <t>Go to https://github.com/marikaris/ChromosomeView/tree/master/test and download the xlsx files from the testFiles directory</t>
+  </si>
+  <si>
+    <t>Make sure d3.js is in the header of MOLGENIS, above jQuery! (I did it above everything)</t>
+  </si>
+  <si>
+    <t>Upload first the questionnaire to MOLGENIS (this is Chr6_vragen_emx_testimport10_met_array.xlsx), then upload the geneData file</t>
+  </si>
+  <si>
+    <t>Now upload the testFiles for all four parts of the questionnaire</t>
+  </si>
+  <si>
+    <t>Make a new tempate and paste the content of the functionality_tabs_v2.ftl file inside the template</t>
+  </si>
+  <si>
+    <t>Name the template as: view-test-entitiesreport.ftl</t>
   </si>
 </sst>
 </file>
@@ -969,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -990,564 +987,565 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" ht="52">
+      <c r="A4" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15">
       <c r="A13" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="26">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="26">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="26">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" ht="26">
       <c r="A20" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="26">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:2" ht="26">
       <c r="A30" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="26">
       <c r="A31" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="26">
       <c r="A32" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="1:2" ht="39">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="26">
       <c r="A34" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B35" s="1"/>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:2" ht="26">
       <c r="A37" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="26">
       <c r="A53" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B61" s="5"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B63" s="3"/>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="26">
       <c r="A71" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="26">
       <c r="A73" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="26">
       <c r="A74" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B78" s="3"/>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="26">
       <c r="A81" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B84" s="3"/>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>